<commit_message>
Started checking the feature identification
For some reason I couln't edit the Jupyter Notebook in my browser. Sorry if I messed anything up by opening the Reddit-MDA file in my local Spyder application again...
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBD84970-1511-4707-9144-8B5FA50E7C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF66D27-C41F-4A6D-BBF9-B80B34FD2549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="103">
   <si>
     <t>Feature</t>
   </si>
@@ -311,13 +322,31 @@
   </si>
   <si>
     <t>Who?</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>3 mistakes in manual coding (corrected and saved as new file), 4 pre-verbal cases that should theoretically be catched by the original code (must be POS-tag errors), 6 post-verbal cases that appear in object position ("What is this?") which are not included in Biber's code (added this in the code). The words in question seem to be tagged as DT most of the time, so I copied the code for finding them into the Determiner-section as well.</t>
+  </si>
+  <si>
+    <t>The words in question seem to be tagged as NN most of the time, so I copied the code for finding them into the Noun-section as well.</t>
+  </si>
+  <si>
+    <t>Instances are not counted because of interjections ("What the fuck is happening"), which we can't really address easily. But features are also not counted because the wh-word is not at the immediate beginning of the sentence - this could be addressed by deleting the sentence-initional criterium (but this way we would also get a lot of junk in probably, such as "I know what will happen")</t>
+  </si>
+  <si>
+    <t>Not found because sentence-final punctuation is apparently deleted at some point in our code. Can we simple delete the command in line 78? (sentence.strip(string.punctuation))</t>
+  </si>
+  <si>
+    <t>Added a missing comma in line 186, but apart from that I can see no reason why these shouldn't be identified. Is there anything wrong with the object "words"? (line 173) - maybe the split-command?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +477,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -794,8 +830,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1150,12 +1188,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J82"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1163,7 +1201,7 @@
     <col min="1" max="1" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1194,8 +1232,11 @@
       <c r="J1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1227,7 +1268,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1259,7 +1300,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1291,7 +1332,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1323,7 +1364,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1355,7 +1396,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -1387,7 +1428,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -1419,39 +1460,42 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.90291262135922301</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
         <v>93</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>10</v>
       </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1483,7 +1527,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1515,7 +1559,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1547,7 +1591,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1579,167 +1623,182 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.87850467289719603</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
         <v>94</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>13</v>
       </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="G14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="K14" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>0.91735537190082606</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
         <v>111</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>10</v>
       </c>
-      <c r="G15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="G15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="K15" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>0.95867768595041303</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
         <v>232</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>10</v>
       </c>
-      <c r="G16" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="G16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="K16" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>0.93506493506493504</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
         <v>144</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>10</v>
       </c>
-      <c r="G17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="K17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>0.96677740863787298</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
+      <c r="C18" s="2">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2">
         <v>291</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>10</v>
       </c>
-      <c r="G18" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="G18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K18" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1771,7 +1830,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1803,7 +1862,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1835,7 +1894,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1867,7 +1926,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1899,7 +1958,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -1931,7 +1990,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -1963,7 +2022,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -1995,7 +2054,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2027,7 +2086,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2059,7 +2118,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2091,7 +2150,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2123,7 +2182,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2155,7 +2214,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Notes from today's meeting
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC1DB0E-B0E9-45D7-AB71-9013DA80A973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5AE72E8-D915-4508-8988-A830C487E8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="495" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
@@ -1197,9 +1197,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated the table for feature identification
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7428B774-0D6A-4C21-B579-43B3AAA0677E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAADEFCE-16F9-4029-9346-3A806E77F36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
   <si>
     <t>Feature</t>
   </si>
@@ -349,7 +349,10 @@
     <t>This is being compiled with the exact code in two functions analyze_particle and analyze_adverb. Could this be causing the problem?</t>
   </si>
   <si>
-    <t>Is being compiled before punctuation is stripped and the regex is working so no idea why it no identifying it</t>
+    <t>line 972: we should not have s-copy() there but another dictionary (or another function nested into it)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">probably the same problem as "hashtag_201" </t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1206,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:J26"/>
+      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,6 +2072,9 @@
       <c r="J26" t="s">
         <v>92</v>
       </c>
+      <c r="K26" s="2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">

</xml_diff>

<commit_message>
Continued checking features, re-wrote code for demonstrative.
I hope everything went well with the versions. For some reason I could no longer see some of the changes I had implemented last month.
</commit_message>
<xml_diff>
--- a/Feature_coding_accuracies_flair_Assignment.xlsx
+++ b/Feature_coding_accuracies_flair_Assignment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ratos\Documents\GitHub\Reddit_MDA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahle\Documents\GitHub\Reddit_MDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAADEFCE-16F9-4029-9346-3A806E77F36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5EE021-19E9-4503-AB9B-EE77FD2C312A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20617" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feature_coding_accuracies_flair" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="111">
   <si>
     <t>Feature</t>
   </si>
@@ -331,9 +333,6 @@
     <t>The words in question seem to be tagged as NN most of the time, so I copied the code for finding them into the Noun-section as well.</t>
   </si>
   <si>
-    <t>Instances are not counted because of interjections ("What the fuck is happening"), which we can't really address easily. But features are also not counted because the wh-word is not at the immediate beginning of the sentence - this could be addressed by deleting the sentence-initional criterium (but this way we would also get a lot of junk in probably, such as "I know what will happen")</t>
-  </si>
-  <si>
     <t>Not found because sentence-final punctuation is apparently deleted at some point in our code. Can we simple delete the command in line 78? (sentence.strip(string.punctuation))</t>
   </si>
   <si>
@@ -353,6 +352,18 @@
   </si>
   <si>
     <t xml:space="preserve">probably the same problem as "hashtag_201" </t>
+  </si>
+  <si>
+    <t>Not found because sentence-final punctuation is apparently deleted at some point in our code. Can we simply delete the command in line 78? (sentence.strip(string.punctuation))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instances are not counted because of interjections ("What the fuck is happening"), which we can't really address easily. But features are also not counted because the wh-word is not at the immediate beginning of the sentence - this could be addressed by deleting the sentence-initional criterium (but this way we would also get a lot of junk in probably, such as "I know what will happen"). </t>
+  </si>
+  <si>
+    <t>Added some more possible cases to our code (e.g. comma following the DO), corrected two mistakes in the manual coding</t>
+  </si>
+  <si>
+    <t>Corrected two mistakes in the manual coding. Added code to allow for one intervening adverb. In most cases the construction is not counted because the form of BE used is &lt;'s&gt; , which we currently do not have in our object [belist], because it can be confused with &lt;'s&gt; as contraction of "has". But: in the constructions for this feature, "has" would mostly be ungrammatical. "that's right" or "it's up in the air". I therefore added code to also count "'s" when occuring within the specific condition. (line 591)</t>
   </si>
 </sst>
 </file>
@@ -849,48 +860,48 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bom" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Célula Vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Ênfase1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Ruim" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -906,7 +917,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1204,17 +1215,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1249,7 +1260,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>73</v>
       </c>
@@ -1281,7 +1292,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1313,7 +1324,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1345,7 +1356,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1377,7 +1388,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -1409,7 +1420,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -1441,7 +1452,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -1473,7 +1484,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>83</v>
       </c>
@@ -1505,10 +1516,10 @@
         <v>95</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -1540,42 +1551,45 @@
         <v>91</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.987788331071913</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>725</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>7</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>0.6</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>0.3</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>0.4</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1607,42 +1621,45 @@
         <v>91</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.8</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>13</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>2</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>69</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>16</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>0.86666666666666603</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>0.44827586206896503</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>0.59090909090909005</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1677,7 +1694,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1712,7 +1729,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1744,10 +1761,10 @@
         <v>91</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
@@ -1779,45 +1796,45 @@
         <v>91</v>
       </c>
       <c r="K17" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.96677740863787298</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>291</v>
+      </c>
+      <c r="F18" s="1">
+        <v>10</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.96677740863787298</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2">
-        <v>291</v>
-      </c>
-      <c r="F18" s="2">
-        <v>10</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1849,7 +1866,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1881,7 +1898,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1913,7 +1930,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -1945,7 +1962,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1977,7 +1994,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2009,7 +2026,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>81</v>
       </c>
@@ -2041,7 +2058,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -2073,10 +2090,10 @@
         <v>92</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2108,7 +2125,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -2140,7 +2157,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2172,7 +2189,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2204,7 +2221,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2236,7 +2253,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2268,7 +2285,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -2300,10 +2317,10 @@
         <v>94</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -2335,10 +2352,10 @@
         <v>94</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2370,7 +2387,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -2402,7 +2419,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2434,7 +2451,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -2466,7 +2483,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -2498,7 +2515,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2530,7 +2547,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -2562,7 +2579,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2594,7 +2611,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -2623,7 +2640,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2652,7 +2669,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -2681,7 +2698,7 @@
         <v>0.66666666666666596</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -2710,7 +2727,7 @@
         <v>0.68965517241379304</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>54</v>
       </c>
@@ -2739,7 +2756,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>25</v>
       </c>
@@ -2768,7 +2785,7 @@
         <v>0.71428571428571397</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -2797,7 +2814,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>87</v>
       </c>
@@ -2826,7 +2843,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -2855,7 +2872,7 @@
         <v>0.76923076923076905</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2884,7 +2901,7 @@
         <v>0.79120879120879095</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>15</v>
       </c>
@@ -2913,7 +2930,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -2942,7 +2959,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -2971,7 +2988,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -3000,7 +3017,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -3029,7 +3046,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -3058,7 +3075,7 @@
         <v>0.81818181818181801</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3087,7 +3104,7 @@
         <v>0.82352941176470495</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -3116,7 +3133,7 @@
         <v>0.83333333333333304</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>71</v>
       </c>
@@ -3145,7 +3162,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>90</v>
       </c>
@@ -3174,7 +3191,7 @@
         <v>0.85714285714285698</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>50</v>
       </c>
@@ -3203,7 +3220,7 @@
         <v>0.86538461538461497</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>53</v>
       </c>
@@ -3232,7 +3249,7 @@
         <v>0.86842105263157798</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -3261,7 +3278,7 @@
         <v>0.86956521739130399</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>12</v>
       </c>
@@ -3290,7 +3307,7 @@
         <v>0.88721804511278102</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -3319,7 +3336,7 @@
         <v>0.88888888888888895</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>60</v>
       </c>
@@ -3348,7 +3365,7 @@
         <v>0.89655172413793105</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -3377,7 +3394,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>64</v>
       </c>
@@ -3406,7 +3423,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>75</v>
       </c>
@@ -3435,7 +3452,7 @@
         <v>0.93333333333333302</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>31</v>
       </c>
@@ -3464,7 +3481,7 @@
         <v>0.94736842105263097</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>62</v>
       </c>
@@ -3493,7 +3510,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>63</v>
       </c>
@@ -3522,7 +3539,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>65</v>
       </c>
@@ -3551,7 +3568,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -3580,7 +3597,7 @@
         <v>0.952380952380952</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3609,7 +3626,7 @@
         <v>0.96428571428571397</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -3638,7 +3655,7 @@
         <v>0.967741935483871</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -3667,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -3696,7 +3713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>27</v>
       </c>
@@ -3725,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>66</v>
       </c>

</xml_diff>